<commit_message>
"CreateClient, SelectVendor,SelectCient should be finished" - Bug and exception testing still needed
</commit_message>
<xml_diff>
--- a/Keele_F_Reed_C-P0/ExcelSheets/ClientList.xlsx
+++ b/Keele_F_Reed_C-P0/ExcelSheets/ClientList.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\P0-Project\Keele_F_Reed_C-P0\Keele_F_Reed_C-P0\ExcelSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F286881D-610C-42FE-B3FF-8D45FEE69ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C6DFD8-409D-4545-853C-9BC3E278206F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="1065" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{A0AD2B87-9B54-4F52-B0DA-953EF1D81E8A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{0F4B5590-EBD4-4140-86EC-D66B824FCF93}"/>
   </bookViews>
   <sheets>
-    <sheet name="Colton" sheetId="2" r:id="rId1"/>
-    <sheet name="Jim" sheetId="6" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
-    <sheet name="Jeff" sheetId="4" r:id="rId4"/>
-    <sheet name="Client info" sheetId="1" r:id="rId5"/>
+    <sheet name="alexander" sheetId="3" r:id="rId1"/>
+    <sheet name="Client info" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,57 +35,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
   <si>
-    <t>Client</t>
+    <t>alexander</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Jeff</t>
-  </si>
-  <si>
-    <t>Jeff@gmail.com</t>
-  </si>
-  <si>
-    <t>Colton</t>
-  </si>
-  <si>
-    <t>Colton@Colton.com</t>
-  </si>
-  <si>
-    <t>Chicken</t>
-  </si>
-  <si>
-    <t>Lettuce</t>
-  </si>
-  <si>
-    <t>Tomatoes</t>
-  </si>
-  <si>
-    <t>Jim</t>
-  </si>
-  <si>
-    <t>jim@jim.com</t>
+    <t>alexander@alexander.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -111,16 +73,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -432,32 +391,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3670D919-96DE-4BB0-8543-722C774904D6}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE2768B2-BD93-4EF5-93F3-CC6D6492073E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6D90464-751E-49A6-9341-F6E1B3DB4F04}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -466,7 +400,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -474,67 +408,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C613642-054E-4321-9BED-A3AB069DB521}">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04DFCFD6-14D5-4802-82C4-2CC2C18F7A5B}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1F98A7-3082-402F-8868-475251BBDC06}">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A32A0B07-F0EE-45C7-B738-F8C4340D703F}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -544,26 +424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{21D8B4D1-3FEF-42AE-A365-C4F410080B91}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>